<commit_message>
feat: Complete CRM modernization - schema migration and UI overhaul
- Migrated lead schema from generic (phone, company) to telecalling fields
  (contact, email, city, university, course, profession)
- Updated status enum to 10 telecalling-specific states
- Redesigned admin dashboard with performance metrics and separate sections
- Overhauled user dashboard with quick actions, filters, and pagination
- Added semantic status badge colors and improved modal UX
- Fixed navigation, escape key handlers, and DOMContentLoaded timing
- Created migration script and updated sample data generator

BREAKING CHANGE: Lead data model and status enum completely replaced
</commit_message>
<xml_diff>
--- a/backend/scripts/sample_leads.xlsx
+++ b/backend/scripts/sample_leads.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:I75"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -407,33 +407,27 @@
         <v>Name</v>
       </c>
       <c r="B1" t="str">
+        <v>Contact</v>
+      </c>
+      <c r="C1" t="str">
         <v>Email</v>
       </c>
-      <c r="C1" t="str">
-        <v>Phone</v>
-      </c>
       <c r="D1" t="str">
-        <v>Contact</v>
+        <v>City</v>
       </c>
       <c r="E1" t="str">
-        <v>City</v>
+        <v>University</v>
       </c>
       <c r="F1" t="str">
-        <v>University</v>
+        <v>Course</v>
       </c>
       <c r="G1" t="str">
-        <v>Course</v>
+        <v>Profession</v>
       </c>
       <c r="H1" t="str">
-        <v>Profession</v>
+        <v>Status</v>
       </c>
       <c r="I1" t="str">
-        <v>Company</v>
-      </c>
-      <c r="J1" t="str">
-        <v>Status</v>
-      </c>
-      <c r="K1" t="str">
         <v>Notes</v>
       </c>
     </row>
@@ -442,33 +436,27 @@
         <v>Alice Johnson</v>
       </c>
       <c r="B2" t="str">
+        <v>+1-202-555-0112</v>
+      </c>
+      <c r="C2" t="str">
         <v>alice@example.com</v>
       </c>
-      <c r="C2" t="str">
-        <v>+1-202-555-0111</v>
-      </c>
       <c r="D2" t="str">
-        <v>+1-202-555-0112</v>
+        <v>New York</v>
       </c>
       <c r="E2" t="str">
-        <v>New York</v>
+        <v>NYU</v>
       </c>
       <c r="F2" t="str">
-        <v>NYU</v>
+        <v>MBA</v>
       </c>
       <c r="G2" t="str">
-        <v>MBA</v>
+        <v>Marketing Manager</v>
       </c>
       <c r="H2" t="str">
-        <v>Marketing Manager</v>
+        <v>Fresh</v>
       </c>
       <c r="I2" t="str">
-        <v>Alpha Corp</v>
-      </c>
-      <c r="J2" t="str">
-        <v>Fresh</v>
-      </c>
-      <c r="K2" t="str">
         <v>Initial inquiry</v>
       </c>
     </row>
@@ -477,33 +465,27 @@
         <v>Bob Singh</v>
       </c>
       <c r="B3" t="str">
+        <v>+1-202-555-0223</v>
+      </c>
+      <c r="C3" t="str">
         <v>bob@example.com</v>
       </c>
-      <c r="C3" t="str">
-        <v>+1-202-555-0222</v>
-      </c>
       <c r="D3" t="str">
-        <v>+1-202-555-0223</v>
+        <v>San Francisco</v>
       </c>
       <c r="E3" t="str">
-        <v>San Francisco</v>
+        <v>Stanford</v>
       </c>
       <c r="F3" t="str">
-        <v>Stanford</v>
+        <v>Data Science</v>
       </c>
       <c r="G3" t="str">
-        <v>Data Science</v>
+        <v>Data Analyst</v>
       </c>
       <c r="H3" t="str">
-        <v>Data Analyst</v>
+        <v>Follow up</v>
       </c>
       <c r="I3" t="str">
-        <v>Beta LLC</v>
-      </c>
-      <c r="J3" t="str">
-        <v>Follow up</v>
-      </c>
-      <c r="K3" t="str">
         <v>Interested in program</v>
       </c>
     </row>
@@ -512,33 +494,27 @@
         <v>Carla Mendes</v>
       </c>
       <c r="B4" t="str">
+        <v>+1-202-555-0334</v>
+      </c>
+      <c r="C4" t="str">
         <v>carla@example.com</v>
       </c>
-      <c r="C4" t="str">
-        <v>+1-202-555-0333</v>
-      </c>
       <c r="D4" t="str">
-        <v>+1-202-555-0334</v>
+        <v>Boston</v>
       </c>
       <c r="E4" t="str">
-        <v>Boston</v>
+        <v>MIT</v>
       </c>
       <c r="F4" t="str">
-        <v>MIT</v>
+        <v>Engineering</v>
       </c>
       <c r="G4" t="str">
-        <v>Engineering</v>
+        <v>Software Engineer</v>
       </c>
       <c r="H4" t="str">
-        <v>Software Engineer</v>
+        <v>Counselled</v>
       </c>
       <c r="I4" t="str">
-        <v>Gamma Industries</v>
-      </c>
-      <c r="J4" t="str">
-        <v>Counselled</v>
-      </c>
-      <c r="K4" t="str">
         <v>Discussed options</v>
       </c>
     </row>
@@ -547,33 +523,27 @@
         <v>David Osei</v>
       </c>
       <c r="B5" t="str">
+        <v>+1-202-555-0445</v>
+      </c>
+      <c r="C5" t="str">
         <v>david@example.com</v>
       </c>
-      <c r="C5" t="str">
-        <v>+1-202-555-0444</v>
-      </c>
       <c r="D5" t="str">
-        <v>+1-202-555-0445</v>
+        <v>Chicago</v>
       </c>
       <c r="E5" t="str">
-        <v>Chicago</v>
+        <v>Northwestern</v>
       </c>
       <c r="F5" t="str">
-        <v>Northwestern</v>
+        <v>Finance</v>
       </c>
       <c r="G5" t="str">
-        <v>Finance</v>
+        <v>Financial Analyst</v>
       </c>
       <c r="H5" t="str">
-        <v>Financial Analyst</v>
+        <v>Request call back</v>
       </c>
       <c r="I5" t="str">
-        <v>Delta Partners</v>
-      </c>
-      <c r="J5" t="str">
-        <v>Request call back</v>
-      </c>
-      <c r="K5" t="str">
         <v>Follow-up needed</v>
       </c>
     </row>
@@ -582,33 +552,27 @@
         <v>Emma Li</v>
       </c>
       <c r="B6" t="str">
+        <v>+1-202-555-0556</v>
+      </c>
+      <c r="C6" t="str">
         <v>emma@example.com</v>
       </c>
-      <c r="C6" t="str">
-        <v>+1-202-555-0555</v>
-      </c>
       <c r="D6" t="str">
-        <v>+1-202-555-0556</v>
+        <v>Seattle</v>
       </c>
       <c r="E6" t="str">
-        <v>Seattle</v>
+        <v>UW</v>
       </c>
       <c r="F6" t="str">
-        <v>UW</v>
+        <v>Computer Science</v>
       </c>
       <c r="G6" t="str">
-        <v>Computer Science</v>
+        <v>Developer</v>
       </c>
       <c r="H6" t="str">
-        <v>Developer</v>
+        <v>Interested in next batch</v>
       </c>
       <c r="I6" t="str">
-        <v>Epsilon Tech</v>
-      </c>
-      <c r="J6" t="str">
-        <v>Interested in next batch</v>
-      </c>
-      <c r="K6" t="str">
         <v>Waiting for schedule</v>
       </c>
     </row>
@@ -617,33 +581,27 @@
         <v>Fahad Khan</v>
       </c>
       <c r="B7" t="str">
+        <v>+1-202-555-0667</v>
+      </c>
+      <c r="C7" t="str">
         <v>fahad@example.com</v>
       </c>
-      <c r="C7" t="str">
-        <v>+1-202-555-0666</v>
-      </c>
       <c r="D7" t="str">
-        <v>+1-202-555-0667</v>
+        <v>Austin</v>
       </c>
       <c r="E7" t="str">
-        <v>Austin</v>
+        <v>UT Austin</v>
       </c>
       <c r="F7" t="str">
-        <v>UT Austin</v>
+        <v>Business</v>
       </c>
       <c r="G7" t="str">
-        <v>Business</v>
+        <v>Business Analyst</v>
       </c>
       <c r="H7" t="str">
-        <v>Business Analyst</v>
+        <v>Registration fees paid</v>
       </c>
       <c r="I7" t="str">
-        <v>Zeta Group</v>
-      </c>
-      <c r="J7" t="str">
-        <v>Registration fees paid</v>
-      </c>
-      <c r="K7" t="str">
         <v>Payment received</v>
       </c>
     </row>
@@ -652,33 +610,27 @@
         <v>Grace Park</v>
       </c>
       <c r="B8" t="str">
+        <v>+1-202-555-0778</v>
+      </c>
+      <c r="C8" t="str">
         <v>grace@example.com</v>
       </c>
-      <c r="C8" t="str">
-        <v>+1-202-555-0777</v>
-      </c>
       <c r="D8" t="str">
-        <v>+1-202-555-0778</v>
+        <v>Los Angeles</v>
       </c>
       <c r="E8" t="str">
-        <v>Los Angeles</v>
+        <v>UCLA</v>
       </c>
       <c r="F8" t="str">
-        <v>UCLA</v>
+        <v>Marketing</v>
       </c>
       <c r="G8" t="str">
-        <v>Marketing</v>
+        <v>Marketing Executive</v>
       </c>
       <c r="H8" t="str">
-        <v>Marketing Executive</v>
+        <v>Enrolled</v>
       </c>
       <c r="I8" t="str">
-        <v>Eta Solutions</v>
-      </c>
-      <c r="J8" t="str">
-        <v>Enrolled</v>
-      </c>
-      <c r="K8" t="str">
         <v>Successfully enrolled</v>
       </c>
     </row>
@@ -687,33 +639,27 @@
         <v>Henry Adams</v>
       </c>
       <c r="B9" t="str">
+        <v>+1-202-555-0889</v>
+      </c>
+      <c r="C9" t="str">
         <v>henry@example.com</v>
       </c>
-      <c r="C9" t="str">
-        <v>+1-202-555-0888</v>
-      </c>
       <c r="D9" t="str">
-        <v>+1-202-555-0889</v>
+        <v>Miami</v>
       </c>
       <c r="E9" t="str">
-        <v>Miami</v>
+        <v>FIU</v>
       </c>
       <c r="F9" t="str">
-        <v>FIU</v>
+        <v>IT</v>
       </c>
       <c r="G9" t="str">
-        <v>IT</v>
+        <v>IT Consultant</v>
       </c>
       <c r="H9" t="str">
-        <v>IT Consultant</v>
+        <v>Buffer fresh</v>
       </c>
       <c r="I9" t="str">
-        <v>Theta Ventures</v>
-      </c>
-      <c r="J9" t="str">
-        <v>Buffer fresh</v>
-      </c>
-      <c r="K9" t="str">
         <v>Pending response</v>
       </c>
     </row>
@@ -722,33 +668,27 @@
         <v>Isabella Cruz</v>
       </c>
       <c r="B10" t="str">
+        <v>+1-202-555-1000</v>
+      </c>
+      <c r="C10" t="str">
         <v>isabella@example.com</v>
       </c>
-      <c r="C10" t="str">
-        <v>+1-202-555-0999</v>
-      </c>
       <c r="D10" t="str">
-        <v>+1-202-555-1000</v>
+        <v>Denver</v>
       </c>
       <c r="E10" t="str">
-        <v>Denver</v>
+        <v>CU Boulder</v>
       </c>
       <c r="F10" t="str">
-        <v>CU Boulder</v>
+        <v>Design</v>
       </c>
       <c r="G10" t="str">
-        <v>Design</v>
+        <v>Designer</v>
       </c>
       <c r="H10" t="str">
-        <v>Designer</v>
+        <v>Did not pick</v>
       </c>
       <c r="I10" t="str">
-        <v>Iota Labs</v>
-      </c>
-      <c r="J10" t="str">
-        <v>Did not pick</v>
-      </c>
-      <c r="K10" t="str">
         <v>No answer</v>
       </c>
     </row>
@@ -757,33 +697,27 @@
         <v>Jack Miller</v>
       </c>
       <c r="B11" t="str">
+        <v>+1-202-555-1001</v>
+      </c>
+      <c r="C11" t="str">
         <v>jack@example.com</v>
       </c>
-      <c r="C11" t="str">
-        <v>+1-202-555-1000</v>
-      </c>
       <c r="D11" t="str">
-        <v>+1-202-555-1001</v>
+        <v>Portland</v>
       </c>
       <c r="E11" t="str">
-        <v>Portland</v>
+        <v>PSU</v>
       </c>
       <c r="F11" t="str">
-        <v>PSU</v>
+        <v>Management</v>
       </c>
       <c r="G11" t="str">
-        <v>Management</v>
+        <v>Manager</v>
       </c>
       <c r="H11" t="str">
-        <v>Manager</v>
+        <v>Junk/not interested</v>
       </c>
       <c r="I11" t="str">
-        <v>Kappa Systems</v>
-      </c>
-      <c r="J11" t="str">
-        <v>Junk/not interested</v>
-      </c>
-      <c r="K11" t="str">
         <v>Not interested</v>
       </c>
     </row>
@@ -792,33 +726,27 @@
         <v>Karen Lopez</v>
       </c>
       <c r="B12" t="str">
+        <v>+1-202-555-1112</v>
+      </c>
+      <c r="C12" t="str">
         <v>karen@example.com</v>
       </c>
-      <c r="C12" t="str">
-        <v>+1-202-555-1111</v>
-      </c>
       <c r="D12" t="str">
-        <v>+1-202-555-1112</v>
+        <v>Phoenix</v>
       </c>
       <c r="E12" t="str">
-        <v>Phoenix</v>
+        <v>ASU</v>
       </c>
       <c r="F12" t="str">
-        <v>ASU</v>
+        <v>Economics</v>
       </c>
       <c r="G12" t="str">
-        <v>Economics</v>
+        <v>Economist</v>
       </c>
       <c r="H12" t="str">
-        <v>Economist</v>
+        <v>Fresh</v>
       </c>
       <c r="I12" t="str">
-        <v>Lambda Consulting</v>
-      </c>
-      <c r="J12" t="str">
-        <v>Fresh</v>
-      </c>
-      <c r="K12" t="str">
         <v>New inquiry</v>
       </c>
     </row>
@@ -827,33 +755,27 @@
         <v>Leo Brown</v>
       </c>
       <c r="B13" t="str">
+        <v>+1-202-555-1223</v>
+      </c>
+      <c r="C13" t="str">
         <v>leo@example.com</v>
       </c>
-      <c r="C13" t="str">
-        <v>+1-202-555-1222</v>
-      </c>
       <c r="D13" t="str">
-        <v>+1-202-555-1223</v>
+        <v>Atlanta</v>
       </c>
       <c r="E13" t="str">
-        <v>Atlanta</v>
+        <v>Georgia Tech</v>
       </c>
       <c r="F13" t="str">
-        <v>Georgia Tech</v>
+        <v>Engineering</v>
       </c>
       <c r="G13" t="str">
-        <v>Engineering</v>
+        <v>Engineer</v>
       </c>
       <c r="H13" t="str">
-        <v>Engineer</v>
+        <v>Counselled</v>
       </c>
       <c r="I13" t="str">
-        <v>Mu Enterprises</v>
-      </c>
-      <c r="J13" t="str">
-        <v>Counselled</v>
-      </c>
-      <c r="K13" t="str">
         <v>Consultation completed</v>
       </c>
     </row>
@@ -862,33 +784,27 @@
         <v>Maya Patel</v>
       </c>
       <c r="B14" t="str">
+        <v>+1-202-555-1334</v>
+      </c>
+      <c r="C14" t="str">
         <v>maya@example.com</v>
       </c>
-      <c r="C14" t="str">
-        <v>+1-202-555-1333</v>
-      </c>
       <c r="D14" t="str">
-        <v>+1-202-555-1334</v>
+        <v>Dallas</v>
       </c>
       <c r="E14" t="str">
-        <v>Dallas</v>
+        <v>SMU</v>
       </c>
       <c r="F14" t="str">
-        <v>SMU</v>
+        <v>MBA</v>
       </c>
       <c r="G14" t="str">
-        <v>MBA</v>
+        <v>Business Owner</v>
       </c>
       <c r="H14" t="str">
-        <v>Business Owner</v>
+        <v>Enrolled</v>
       </c>
       <c r="I14" t="str">
-        <v>Nu Technologies</v>
-      </c>
-      <c r="J14" t="str">
-        <v>Enrolled</v>
-      </c>
-      <c r="K14" t="str">
         <v>Enrolled successfully</v>
       </c>
     </row>
@@ -897,33 +813,27 @@
         <v>Noah Kim</v>
       </c>
       <c r="B15" t="str">
+        <v>+1-202-555-1445</v>
+      </c>
+      <c r="C15" t="str">
         <v>noah@example.com</v>
       </c>
-      <c r="C15" t="str">
-        <v>+1-202-555-1444</v>
-      </c>
       <c r="D15" t="str">
-        <v>+1-202-555-1445</v>
+        <v>Philadelphia</v>
       </c>
       <c r="E15" t="str">
-        <v>Philadelphia</v>
+        <v>UPenn</v>
       </c>
       <c r="F15" t="str">
-        <v>UPenn</v>
+        <v>Finance</v>
       </c>
       <c r="G15" t="str">
-        <v>Finance</v>
+        <v>Accountant</v>
       </c>
       <c r="H15" t="str">
-        <v>Accountant</v>
+        <v>Follow up</v>
       </c>
       <c r="I15" t="str">
-        <v>Xi Innovations</v>
-      </c>
-      <c r="J15" t="str">
-        <v>Follow up</v>
-      </c>
-      <c r="K15" t="str">
         <v>Needs follow up</v>
       </c>
     </row>
@@ -932,39 +842,1744 @@
         <v>Olivia Chen</v>
       </c>
       <c r="B16" t="str">
+        <v>+1-202-555-1556</v>
+      </c>
+      <c r="C16" t="str">
         <v>olivia@example.com</v>
       </c>
-      <c r="C16" t="str">
-        <v>+1-202-555-1555</v>
-      </c>
       <c r="D16" t="str">
-        <v>+1-202-555-1556</v>
+        <v>San Diego</v>
       </c>
       <c r="E16" t="str">
-        <v>San Diego</v>
+        <v>UCSD</v>
       </c>
       <c r="F16" t="str">
-        <v>UCSD</v>
+        <v>Biology</v>
       </c>
       <c r="G16" t="str">
+        <v>Researcher</v>
+      </c>
+      <c r="H16" t="str">
+        <v>Fresh</v>
+      </c>
+      <c r="I16" t="str">
+        <v>First contact</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>Paul Rivera</v>
+      </c>
+      <c r="B17" t="str">
+        <v>+1-202-555-2001</v>
+      </c>
+      <c r="C17" t="str">
+        <v>paul@example.com</v>
+      </c>
+      <c r="D17" t="str">
+        <v>Houston</v>
+      </c>
+      <c r="E17" t="str">
+        <v>Rice</v>
+      </c>
+      <c r="F17" t="str">
+        <v>MBA</v>
+      </c>
+      <c r="G17" t="str">
+        <v>Consultant</v>
+      </c>
+      <c r="H17" t="str">
+        <v>Fresh</v>
+      </c>
+      <c r="I17" t="str">
+        <v>New inquiry</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>Sophia Turner</v>
+      </c>
+      <c r="B18" t="str">
+        <v>+1-202-555-2002</v>
+      </c>
+      <c r="C18" t="str">
+        <v>sophia@example.com</v>
+      </c>
+      <c r="D18" t="str">
+        <v>Las Vegas</v>
+      </c>
+      <c r="E18" t="str">
+        <v>UNLV</v>
+      </c>
+      <c r="F18" t="str">
+        <v>Hospitality</v>
+      </c>
+      <c r="G18" t="str">
+        <v>Hotel Manager</v>
+      </c>
+      <c r="H18" t="str">
+        <v>Follow up</v>
+      </c>
+      <c r="I18" t="str">
+        <v>Requested brochure</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>Marcus Green</v>
+      </c>
+      <c r="B19" t="str">
+        <v>+1-202-555-2003</v>
+      </c>
+      <c r="C19" t="str">
+        <v>marcus@example.com</v>
+      </c>
+      <c r="D19" t="str">
+        <v>Detroit</v>
+      </c>
+      <c r="E19" t="str">
+        <v>Wayne State</v>
+      </c>
+      <c r="F19" t="str">
+        <v>Engineering</v>
+      </c>
+      <c r="G19" t="str">
+        <v>Mechanical Engineer</v>
+      </c>
+      <c r="H19" t="str">
+        <v>Counselled</v>
+      </c>
+      <c r="I19" t="str">
+        <v>Discussed career path</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>Natalie Brooks</v>
+      </c>
+      <c r="B20" t="str">
+        <v>+1-202-555-2004</v>
+      </c>
+      <c r="C20" t="str">
+        <v>natalie@example.com</v>
+      </c>
+      <c r="D20" t="str">
+        <v>Charlotte</v>
+      </c>
+      <c r="E20" t="str">
+        <v>UNC Charlotte</v>
+      </c>
+      <c r="F20" t="str">
+        <v>Finance</v>
+      </c>
+      <c r="G20" t="str">
+        <v>Banker</v>
+      </c>
+      <c r="H20" t="str">
+        <v>Request call back</v>
+      </c>
+      <c r="I20" t="str">
+        <v>Asked for details</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>Omar Hassan</v>
+      </c>
+      <c r="B21" t="str">
+        <v>+1-202-555-2005</v>
+      </c>
+      <c r="C21" t="str">
+        <v>omar@example.com</v>
+      </c>
+      <c r="D21" t="str">
+        <v>Orlando</v>
+      </c>
+      <c r="E21" t="str">
+        <v>UCF</v>
+      </c>
+      <c r="F21" t="str">
+        <v>Computer Science</v>
+      </c>
+      <c r="G21" t="str">
+        <v>Software Developer</v>
+      </c>
+      <c r="H21" t="str">
+        <v>Interested in next batch</v>
+      </c>
+      <c r="I21" t="str">
+        <v>Waiting for schedule</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>Priya Sharma</v>
+      </c>
+      <c r="B22" t="str">
+        <v>+1-202-555-2006</v>
+      </c>
+      <c r="C22" t="str">
+        <v>priya@example.com</v>
+      </c>
+      <c r="D22" t="str">
+        <v>San Jose</v>
+      </c>
+      <c r="E22" t="str">
+        <v>SJSU</v>
+      </c>
+      <c r="F22" t="str">
+        <v>Business</v>
+      </c>
+      <c r="G22" t="str">
+        <v>Entrepreneur</v>
+      </c>
+      <c r="H22" t="str">
+        <v>Registration fees paid</v>
+      </c>
+      <c r="I22" t="str">
+        <v>Payment confirmed</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>Quentin Blake</v>
+      </c>
+      <c r="B23" t="str">
+        <v>+1-202-555-2007</v>
+      </c>
+      <c r="C23" t="str">
+        <v>quentin@example.com</v>
+      </c>
+      <c r="D23" t="str">
+        <v>Minneapolis</v>
+      </c>
+      <c r="E23" t="str">
+        <v>UMN</v>
+      </c>
+      <c r="F23" t="str">
+        <v>Marketing</v>
+      </c>
+      <c r="G23" t="str">
+        <v>Brand Strategist</v>
+      </c>
+      <c r="H23" t="str">
+        <v>Enrolled</v>
+      </c>
+      <c r="I23" t="str">
+        <v>Joined program</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>Rosa Martinez</v>
+      </c>
+      <c r="B24" t="str">
+        <v>+1-202-555-2008</v>
+      </c>
+      <c r="C24" t="str">
+        <v>rosa@example.com</v>
+      </c>
+      <c r="D24" t="str">
+        <v>Tampa</v>
+      </c>
+      <c r="E24" t="str">
+        <v>USF</v>
+      </c>
+      <c r="F24" t="str">
         <v>Biology</v>
       </c>
-      <c r="H16" t="str">
+      <c r="G24" t="str">
+        <v>Lab Technician</v>
+      </c>
+      <c r="H24" t="str">
+        <v>Buffer fresh</v>
+      </c>
+      <c r="I24" t="str">
+        <v>Pending confirmation</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>Samuel Wright</v>
+      </c>
+      <c r="B25" t="str">
+        <v>+1-202-555-2009</v>
+      </c>
+      <c r="C25" t="str">
+        <v>samuel@example.com</v>
+      </c>
+      <c r="D25" t="str">
+        <v>Cleveland</v>
+      </c>
+      <c r="E25" t="str">
+        <v>Case Western</v>
+      </c>
+      <c r="F25" t="str">
+        <v>Law</v>
+      </c>
+      <c r="G25" t="str">
+        <v>Legal Assistant</v>
+      </c>
+      <c r="H25" t="str">
+        <v>Did not pick</v>
+      </c>
+      <c r="I25" t="str">
+        <v>No response</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>Tina Zhang</v>
+      </c>
+      <c r="B26" t="str">
+        <v>+1-202-555-2010</v>
+      </c>
+      <c r="C26" t="str">
+        <v>tina@example.com</v>
+      </c>
+      <c r="D26" t="str">
+        <v>Salt Lake City</v>
+      </c>
+      <c r="E26" t="str">
+        <v>U of Utah</v>
+      </c>
+      <c r="F26" t="str">
+        <v>Design</v>
+      </c>
+      <c r="G26" t="str">
+        <v>Graphic Designer</v>
+      </c>
+      <c r="H26" t="str">
+        <v>Junk/not interested</v>
+      </c>
+      <c r="I26" t="str">
+        <v>Not interested</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>Usha Nair</v>
+      </c>
+      <c r="B27" t="str">
+        <v>+1-202-555-2011</v>
+      </c>
+      <c r="C27" t="str">
+        <v>usha@example.com</v>
+      </c>
+      <c r="D27" t="str">
+        <v>Baltimore</v>
+      </c>
+      <c r="E27" t="str">
+        <v>Johns Hopkins</v>
+      </c>
+      <c r="F27" t="str">
+        <v>Medicine</v>
+      </c>
+      <c r="G27" t="str">
+        <v>Doctor</v>
+      </c>
+      <c r="H27" t="str">
+        <v>Fresh</v>
+      </c>
+      <c r="I27" t="str">
+        <v>Initial inquiry</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>Victor Hugo</v>
+      </c>
+      <c r="B28" t="str">
+        <v>+1-202-555-2012</v>
+      </c>
+      <c r="C28" t="str">
+        <v>victor@example.com</v>
+      </c>
+      <c r="D28" t="str">
+        <v>Kansas City</v>
+      </c>
+      <c r="E28" t="str">
+        <v>UMKC</v>
+      </c>
+      <c r="F28" t="str">
+        <v>Economics</v>
+      </c>
+      <c r="G28" t="str">
+        <v>Economist</v>
+      </c>
+      <c r="H28" t="str">
+        <v>Counselled</v>
+      </c>
+      <c r="I28" t="str">
+        <v>Consultation done</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>Wendy Scott</v>
+      </c>
+      <c r="B29" t="str">
+        <v>+1-202-555-2013</v>
+      </c>
+      <c r="C29" t="str">
+        <v>wendy@example.com</v>
+      </c>
+      <c r="D29" t="str">
+        <v>Columbus</v>
+      </c>
+      <c r="E29" t="str">
+        <v>OSU</v>
+      </c>
+      <c r="F29" t="str">
+        <v>Psychology</v>
+      </c>
+      <c r="G29" t="str">
+        <v>Therapist</v>
+      </c>
+      <c r="H29" t="str">
+        <v>Enrolled</v>
+      </c>
+      <c r="I29" t="str">
+        <v>Joined successfully</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>Xavier Lopez</v>
+      </c>
+      <c r="B30" t="str">
+        <v>+1-202-555-2014</v>
+      </c>
+      <c r="C30" t="str">
+        <v>xavier@example.com</v>
+      </c>
+      <c r="D30" t="str">
+        <v>Indianapolis</v>
+      </c>
+      <c r="E30" t="str">
+        <v>IUPUI</v>
+      </c>
+      <c r="F30" t="str">
+        <v>IT</v>
+      </c>
+      <c r="G30" t="str">
+        <v>IT Specialist</v>
+      </c>
+      <c r="H30" t="str">
+        <v>Follow up</v>
+      </c>
+      <c r="I30" t="str">
+        <v>Needs more info</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>Yara Ali</v>
+      </c>
+      <c r="B31" t="str">
+        <v>+1-202-555-2015</v>
+      </c>
+      <c r="C31" t="str">
+        <v>yara@example.com</v>
+      </c>
+      <c r="D31" t="str">
+        <v>St. Louis</v>
+      </c>
+      <c r="E31" t="str">
+        <v>WashU</v>
+      </c>
+      <c r="F31" t="str">
+        <v>Architecture</v>
+      </c>
+      <c r="G31" t="str">
+        <v>Architect</v>
+      </c>
+      <c r="H31" t="str">
+        <v>Fresh</v>
+      </c>
+      <c r="I31" t="str">
+        <v>First contact</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>Zane Carter</v>
+      </c>
+      <c r="B32" t="str">
+        <v>+1-202-555-2016</v>
+      </c>
+      <c r="C32" t="str">
+        <v>zane@example.com</v>
+      </c>
+      <c r="D32" t="str">
+        <v>Milwaukee</v>
+      </c>
+      <c r="E32" t="str">
+        <v>Marquette</v>
+      </c>
+      <c r="F32" t="str">
+        <v>Engineering</v>
+      </c>
+      <c r="G32" t="str">
+        <v>Civil Engineer</v>
+      </c>
+      <c r="H32" t="str">
+        <v>Request call back</v>
+      </c>
+      <c r="I32" t="str">
+        <v>Asked for callback</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>Amira Khan</v>
+      </c>
+      <c r="B33" t="str">
+        <v>+1-202-555-2017</v>
+      </c>
+      <c r="C33" t="str">
+        <v>amira@example.com</v>
+      </c>
+      <c r="D33" t="str">
+        <v>Raleigh</v>
+      </c>
+      <c r="E33" t="str">
+        <v>NC State</v>
+      </c>
+      <c r="F33" t="str">
+        <v>Data Science</v>
+      </c>
+      <c r="G33" t="str">
+        <v>Data Scientist</v>
+      </c>
+      <c r="H33" t="str">
+        <v>Interested in next batch</v>
+      </c>
+      <c r="I33" t="str">
+        <v>Waiting for schedule</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>Brian Lee</v>
+      </c>
+      <c r="B34" t="str">
+        <v>+1-202-555-2018</v>
+      </c>
+      <c r="C34" t="str">
+        <v>brian@example.com</v>
+      </c>
+      <c r="D34" t="str">
+        <v>Sacramento</v>
+      </c>
+      <c r="E34" t="str">
+        <v>CSUS</v>
+      </c>
+      <c r="F34" t="str">
+        <v>Business</v>
+      </c>
+      <c r="G34" t="str">
+        <v>Business Consultant</v>
+      </c>
+      <c r="H34" t="str">
+        <v>Registration fees paid</v>
+      </c>
+      <c r="I34" t="str">
+        <v>Payment received</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>Clara Gomez</v>
+      </c>
+      <c r="B35" t="str">
+        <v>+1-202-555-2019</v>
+      </c>
+      <c r="C35" t="str">
+        <v>clara@example.com</v>
+      </c>
+      <c r="D35" t="str">
+        <v>San Antonio</v>
+      </c>
+      <c r="E35" t="str">
+        <v>UTSA</v>
+      </c>
+      <c r="F35" t="str">
+        <v>Marketing</v>
+      </c>
+      <c r="G35" t="str">
+        <v>Marketing Specialist</v>
+      </c>
+      <c r="H35" t="str">
+        <v>Enrolled</v>
+      </c>
+      <c r="I35" t="str">
+        <v>Enrolled successfully</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>Derek White</v>
+      </c>
+      <c r="B36" t="str">
+        <v>+1-202-555-2020</v>
+      </c>
+      <c r="C36" t="str">
+        <v>derek@example.com</v>
+      </c>
+      <c r="D36" t="str">
+        <v>Nashville</v>
+      </c>
+      <c r="E36" t="str">
+        <v>Vanderbilt</v>
+      </c>
+      <c r="F36" t="str">
+        <v>Music</v>
+      </c>
+      <c r="G36" t="str">
+        <v>Musician</v>
+      </c>
+      <c r="H36" t="str">
+        <v>Buffer fresh</v>
+      </c>
+      <c r="I36" t="str">
+        <v>Pending response</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>Elena Petrova</v>
+      </c>
+      <c r="B37" t="str">
+        <v>+1-202-555-2021</v>
+      </c>
+      <c r="C37" t="str">
+        <v>elena@example.com</v>
+      </c>
+      <c r="D37" t="str">
+        <v>Pittsburgh</v>
+      </c>
+      <c r="E37" t="str">
+        <v>CMU</v>
+      </c>
+      <c r="F37" t="str">
+        <v>Robotics</v>
+      </c>
+      <c r="G37" t="str">
+        <v>Robotics Engineer</v>
+      </c>
+      <c r="H37" t="str">
+        <v>Counselled</v>
+      </c>
+      <c r="I37" t="str">
+        <v>Discussed options</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>Felix Brown</v>
+      </c>
+      <c r="B38" t="str">
+        <v>+1-202-555-2022</v>
+      </c>
+      <c r="C38" t="str">
+        <v>felix@example.com</v>
+      </c>
+      <c r="D38" t="str">
+        <v>Cincinnati</v>
+      </c>
+      <c r="E38" t="str">
+        <v>UC</v>
+      </c>
+      <c r="F38" t="str">
+        <v>Chemistry</v>
+      </c>
+      <c r="G38" t="str">
+        <v>Chemist</v>
+      </c>
+      <c r="H38" t="str">
+        <v>Follow up</v>
+      </c>
+      <c r="I38" t="str">
+        <v>Interested in program</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>Gina Torres</v>
+      </c>
+      <c r="B39" t="str">
+        <v>+1-202-555-2023</v>
+      </c>
+      <c r="C39" t="str">
+        <v>gina@example.com</v>
+      </c>
+      <c r="D39" t="str">
+        <v>Buffalo</v>
+      </c>
+      <c r="E39" t="str">
+        <v>UB</v>
+      </c>
+      <c r="F39" t="str">
+        <v>Law</v>
+      </c>
+      <c r="G39" t="str">
+        <v>Lawyer</v>
+      </c>
+      <c r="H39" t="str">
+        <v>Fresh</v>
+      </c>
+      <c r="I39" t="str">
+        <v>Initial inquiry</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>Hector Ramirez</v>
+      </c>
+      <c r="B40" t="str">
+        <v>+1-202-555-2024</v>
+      </c>
+      <c r="C40" t="str">
+        <v>hector@example.com</v>
+      </c>
+      <c r="D40" t="str">
+        <v>Richmond</v>
+      </c>
+      <c r="E40" t="str">
+        <v>VCU</v>
+      </c>
+      <c r="F40" t="str">
+        <v>Finance</v>
+      </c>
+      <c r="G40" t="str">
+        <v>Financial Advisor</v>
+      </c>
+      <c r="H40" t="str">
+        <v>Request call back</v>
+      </c>
+      <c r="I40" t="str">
+        <v>Follow-up needed</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>Ivy Chen</v>
+      </c>
+      <c r="B41" t="str">
+        <v>+1-202-555-2025</v>
+      </c>
+      <c r="C41" t="str">
+        <v>ivy@example.com</v>
+      </c>
+      <c r="D41" t="str">
+        <v>Hartford</v>
+      </c>
+      <c r="E41" t="str">
+        <v>UConn</v>
+      </c>
+      <c r="F41" t="str">
+        <v>Biology</v>
+      </c>
+      <c r="G41" t="str">
+        <v>Research Assistant</v>
+      </c>
+      <c r="H41" t="str">
+        <v>Interested in next batch</v>
+      </c>
+      <c r="I41" t="str">
+        <v>Waiting for schedule</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>James Bond</v>
+      </c>
+      <c r="B42" t="str">
+        <v>+1-202-555-2026</v>
+      </c>
+      <c r="C42" t="str">
+        <v>james@example.com</v>
+      </c>
+      <c r="D42" t="str">
+        <v>Anchorage</v>
+      </c>
+      <c r="E42" t="str">
+        <v>UAA</v>
+      </c>
+      <c r="F42" t="str">
+        <v>Criminology</v>
+      </c>
+      <c r="G42" t="str">
+        <v>Investigator</v>
+      </c>
+      <c r="H42" t="str">
+        <v>Junk/not interested</v>
+      </c>
+      <c r="I42" t="str">
+        <v>Not interested</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>Kylie Morgan</v>
+      </c>
+      <c r="B43" t="str">
+        <v>+1-202-555-2027</v>
+      </c>
+      <c r="C43" t="str">
+        <v>kylie@example.com</v>
+      </c>
+      <c r="D43" t="str">
+        <v>Boise</v>
+      </c>
+      <c r="E43" t="str">
+        <v>BSU</v>
+      </c>
+      <c r="F43" t="str">
+        <v>Education</v>
+      </c>
+      <c r="G43" t="str">
+        <v>Teacher</v>
+      </c>
+      <c r="H43" t="str">
+        <v>Fresh</v>
+      </c>
+      <c r="I43" t="str">
+        <v>New inquiry</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>Liam Davis</v>
+      </c>
+      <c r="B44" t="str">
+        <v>+1-202-555-2028</v>
+      </c>
+      <c r="C44" t="str">
+        <v>liam@example.com</v>
+      </c>
+      <c r="D44" t="str">
+        <v>Madison</v>
+      </c>
+      <c r="E44" t="str">
+        <v>UW Madison</v>
+      </c>
+      <c r="F44" t="str">
+        <v>Economics</v>
+      </c>
+      <c r="G44" t="str">
+        <v>Economist</v>
+      </c>
+      <c r="H44" t="str">
+        <v>Counselled</v>
+      </c>
+      <c r="I44" t="str">
+        <v>Consultation completed</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>Mila Novak</v>
+      </c>
+      <c r="B45" t="str">
+        <v>+1-202-555-2029</v>
+      </c>
+      <c r="C45" t="str">
+        <v>mila@example.com</v>
+      </c>
+      <c r="D45" t="str">
+        <v>Albany</v>
+      </c>
+      <c r="E45" t="str">
+        <v>SUNY Albany</v>
+      </c>
+      <c r="F45" t="str">
+        <v>Political Science</v>
+      </c>
+      <c r="G45" t="str">
+        <v>Policy Analyst</v>
+      </c>
+      <c r="H45" t="str">
+        <v>Enrolled</v>
+      </c>
+      <c r="I45" t="str">
+        <v>Enrolled successfully</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>Nate Robinson</v>
+      </c>
+      <c r="B46" t="str">
+        <v>+1-202-555-2030</v>
+      </c>
+      <c r="C46" t="str">
+        <v>nate@example.com</v>
+      </c>
+      <c r="D46" t="str">
+        <v>Des Moines</v>
+      </c>
+      <c r="E46" t="str">
+        <v>Drake</v>
+      </c>
+      <c r="F46" t="str">
+        <v>Management</v>
+      </c>
+      <c r="G46" t="str">
+        <v>Manager</v>
+      </c>
+      <c r="H46" t="str">
+        <v>Follow up</v>
+      </c>
+      <c r="I46" t="str">
+        <v>Pending meeting</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>Olga Ivanova</v>
+      </c>
+      <c r="B47" t="str">
+        <v>+1-202-555-2031</v>
+      </c>
+      <c r="C47" t="str">
+        <v>olga@example.com</v>
+      </c>
+      <c r="D47" t="str">
+        <v>Spokane</v>
+      </c>
+      <c r="E47" t="str">
+        <v>WSU</v>
+      </c>
+      <c r="F47" t="str">
+        <v>Nursing</v>
+      </c>
+      <c r="G47" t="str">
+        <v>Nurse</v>
+      </c>
+      <c r="H47" t="str">
+        <v>Fresh</v>
+      </c>
+      <c r="I47" t="str">
+        <v>Initial inquiry</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>Peter Wang</v>
+      </c>
+      <c r="B48" t="str">
+        <v>+1-202-555-2032</v>
+      </c>
+      <c r="C48" t="str">
+        <v>peter@example.com</v>
+      </c>
+      <c r="D48" t="str">
+        <v>New Orleans</v>
+      </c>
+      <c r="E48" t="str">
+        <v>Tulane</v>
+      </c>
+      <c r="F48" t="str">
+        <v>Public Health</v>
+      </c>
+      <c r="G48" t="str">
+        <v>Coordinator</v>
+      </c>
+      <c r="H48" t="str">
+        <v>Counselled</v>
+      </c>
+      <c r="I48" t="str">
+        <v>Explored syllabus</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>Queenie Das</v>
+      </c>
+      <c r="B49" t="str">
+        <v>+1-202-555-2033</v>
+      </c>
+      <c r="C49" t="str">
+        <v>queenie@example.com</v>
+      </c>
+      <c r="D49" t="str">
+        <v>Omaha</v>
+      </c>
+      <c r="E49" t="str">
+        <v>UNO</v>
+      </c>
+      <c r="F49" t="str">
+        <v>Accounting</v>
+      </c>
+      <c r="G49" t="str">
+        <v>Auditor</v>
+      </c>
+      <c r="H49" t="str">
+        <v>Enrolled</v>
+      </c>
+      <c r="I49" t="str">
+        <v>Onboarded</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>Rafael Costa</v>
+      </c>
+      <c r="B50" t="str">
+        <v>+1-202-555-2034</v>
+      </c>
+      <c r="C50" t="str">
+        <v>rafael@example.com</v>
+      </c>
+      <c r="D50" t="str">
+        <v>El Paso</v>
+      </c>
+      <c r="E50" t="str">
+        <v>UTEP</v>
+      </c>
+      <c r="F50" t="str">
+        <v>Engineering</v>
+      </c>
+      <c r="G50" t="str">
+        <v>Electrical Engineer</v>
+      </c>
+      <c r="H50" t="str">
+        <v>Buffer fresh</v>
+      </c>
+      <c r="I50" t="str">
+        <v>Awaiting reply</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>Sara Ahmed</v>
+      </c>
+      <c r="B51" t="str">
+        <v>+1-202-555-2035</v>
+      </c>
+      <c r="C51" t="str">
+        <v>sara@example.com</v>
+      </c>
+      <c r="D51" t="str">
+        <v>Fresno</v>
+      </c>
+      <c r="E51" t="str">
+        <v>Fresno State</v>
+      </c>
+      <c r="F51" t="str">
+        <v>Agriculture</v>
+      </c>
+      <c r="G51" t="str">
+        <v>Ag Specialist</v>
+      </c>
+      <c r="H51" t="str">
+        <v>Request call back</v>
+      </c>
+      <c r="I51" t="str">
+        <v>Preferred afternoon call</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>Tom Baker</v>
+      </c>
+      <c r="B52" t="str">
+        <v>+1-202-555-2036</v>
+      </c>
+      <c r="C52" t="str">
+        <v>tom@example.com</v>
+      </c>
+      <c r="D52" t="str">
+        <v>Reno</v>
+      </c>
+      <c r="E52" t="str">
+        <v>UNR</v>
+      </c>
+      <c r="F52" t="str">
+        <v>Computer Science</v>
+      </c>
+      <c r="G52" t="str">
+        <v>Backend Developer</v>
+      </c>
+      <c r="H52" t="str">
+        <v>Interested in next batch</v>
+      </c>
+      <c r="I52" t="str">
+        <v>Waiting next intake</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>Uma Kapoor</v>
+      </c>
+      <c r="B53" t="str">
+        <v>+1-202-555-2037</v>
+      </c>
+      <c r="C53" t="str">
+        <v>uma@example.com</v>
+      </c>
+      <c r="D53" t="str">
+        <v>Birmingham</v>
+      </c>
+      <c r="E53" t="str">
+        <v>UAB</v>
+      </c>
+      <c r="F53" t="str">
+        <v>Biotech</v>
+      </c>
+      <c r="G53" t="str">
         <v>Researcher</v>
       </c>
-      <c r="I16" t="str">
-        <v>Omicron Global</v>
-      </c>
-      <c r="J16" t="str">
+      <c r="H53" t="str">
+        <v>Registration fees paid</v>
+      </c>
+      <c r="I53" t="str">
+        <v>Payment verified</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>Vikram Iyer</v>
+      </c>
+      <c r="B54" t="str">
+        <v>+1-202-555-2038</v>
+      </c>
+      <c r="C54" t="str">
+        <v>vikram@example.com</v>
+      </c>
+      <c r="D54" t="str">
+        <v>Tulsa</v>
+      </c>
+      <c r="E54" t="str">
+        <v>TU</v>
+      </c>
+      <c r="F54" t="str">
+        <v>Energy</v>
+      </c>
+      <c r="G54" t="str">
+        <v>Energy Analyst</v>
+      </c>
+      <c r="H54" t="str">
+        <v>Follow up</v>
+      </c>
+      <c r="I54" t="str">
+        <v>Requested case studies</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>Will Harper</v>
+      </c>
+      <c r="B55" t="str">
+        <v>+1-202-555-2039</v>
+      </c>
+      <c r="C55" t="str">
+        <v>will@example.com</v>
+      </c>
+      <c r="D55" t="str">
+        <v>Wichita</v>
+      </c>
+      <c r="E55" t="str">
+        <v>WSU</v>
+      </c>
+      <c r="F55" t="str">
+        <v>Aviation</v>
+      </c>
+      <c r="G55" t="str">
+        <v>Pilot</v>
+      </c>
+      <c r="H55" t="str">
         <v>Fresh</v>
       </c>
-      <c r="K16" t="str">
+      <c r="I55" t="str">
         <v>First contact</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>Xenia Morales</v>
+      </c>
+      <c r="B56" t="str">
+        <v>+1-202-555-2040</v>
+      </c>
+      <c r="C56" t="str">
+        <v>xenia@example.com</v>
+      </c>
+      <c r="D56" t="str">
+        <v>Baton Rouge</v>
+      </c>
+      <c r="E56" t="str">
+        <v>LSU</v>
+      </c>
+      <c r="F56" t="str">
+        <v>Chemistry</v>
+      </c>
+      <c r="G56" t="str">
+        <v>Lab Assistant</v>
+      </c>
+      <c r="H56" t="str">
+        <v>Counselled</v>
+      </c>
+      <c r="I56" t="str">
+        <v>Compared programs</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>Yusuf Khan</v>
+      </c>
+      <c r="B57" t="str">
+        <v>+1-202-555-2041</v>
+      </c>
+      <c r="C57" t="str">
+        <v>yusuf@example.com</v>
+      </c>
+      <c r="D57" t="str">
+        <v>Lexington</v>
+      </c>
+      <c r="E57" t="str">
+        <v>UK</v>
+      </c>
+      <c r="F57" t="str">
+        <v>Statistics</v>
+      </c>
+      <c r="G57" t="str">
+        <v>Statistician</v>
+      </c>
+      <c r="H57" t="str">
+        <v>Enrolled</v>
+      </c>
+      <c r="I57" t="str">
+        <v>Confirmed enrollment</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>Zara Patel</v>
+      </c>
+      <c r="B58" t="str">
+        <v>+1-202-555-2042</v>
+      </c>
+      <c r="C58" t="str">
+        <v>zara@example.com</v>
+      </c>
+      <c r="D58" t="str">
+        <v>Lincoln</v>
+      </c>
+      <c r="E58" t="str">
+        <v>UNL</v>
+      </c>
+      <c r="F58" t="str">
+        <v>Psychology</v>
+      </c>
+      <c r="G58" t="str">
+        <v>Counselor</v>
+      </c>
+      <c r="H58" t="str">
+        <v>Buffer fresh</v>
+      </c>
+      <c r="I58" t="str">
+        <v>Pending confirmation</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>Aiden Clark</v>
+      </c>
+      <c r="B59" t="str">
+        <v>+1-202-555-2043</v>
+      </c>
+      <c r="C59" t="str">
+        <v>aiden@example.com</v>
+      </c>
+      <c r="D59" t="str">
+        <v>Plano</v>
+      </c>
+      <c r="E59" t="str">
+        <v>UTD</v>
+      </c>
+      <c r="F59" t="str">
+        <v>IT</v>
+      </c>
+      <c r="G59" t="str">
+        <v>Systems Admin</v>
+      </c>
+      <c r="H59" t="str">
+        <v>Did not pick</v>
+      </c>
+      <c r="I59" t="str">
+        <v>Missed call</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>Bella Rossi</v>
+      </c>
+      <c r="B60" t="str">
+        <v>+1-202-555-2044</v>
+      </c>
+      <c r="C60" t="str">
+        <v>bella@example.com</v>
+      </c>
+      <c r="D60" t="str">
+        <v>Chandler</v>
+      </c>
+      <c r="E60" t="str">
+        <v>ASU</v>
+      </c>
+      <c r="F60" t="str">
+        <v>Design</v>
+      </c>
+      <c r="G60" t="str">
+        <v>UI Designer</v>
+      </c>
+      <c r="H60" t="str">
+        <v>Junk/not interested</v>
+      </c>
+      <c r="I60" t="str">
+        <v>Not a fit</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>Carlos Ortega</v>
+      </c>
+      <c r="B61" t="str">
+        <v>+1-202-555-2045</v>
+      </c>
+      <c r="C61" t="str">
+        <v>carlos@example.com</v>
+      </c>
+      <c r="D61" t="str">
+        <v>Glendale</v>
+      </c>
+      <c r="E61" t="str">
+        <v>NAU</v>
+      </c>
+      <c r="F61" t="str">
+        <v>Business</v>
+      </c>
+      <c r="G61" t="str">
+        <v>Sales Lead</v>
+      </c>
+      <c r="H61" t="str">
+        <v>Fresh</v>
+      </c>
+      <c r="I61" t="str">
+        <v>New inquiry</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>Diana Prince</v>
+      </c>
+      <c r="B62" t="str">
+        <v>+1-202-555-2046</v>
+      </c>
+      <c r="C62" t="str">
+        <v>diana@example.com</v>
+      </c>
+      <c r="D62" t="str">
+        <v>Irving</v>
+      </c>
+      <c r="E62" t="str">
+        <v>UT Arlington</v>
+      </c>
+      <c r="F62" t="str">
+        <v>Management</v>
+      </c>
+      <c r="G62" t="str">
+        <v>Operations Lead</v>
+      </c>
+      <c r="H62" t="str">
+        <v>Follow up</v>
+      </c>
+      <c r="I62" t="str">
+        <v>Requested curriculum</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>Ethan Young</v>
+      </c>
+      <c r="B63" t="str">
+        <v>+1-202-555-2047</v>
+      </c>
+      <c r="C63" t="str">
+        <v>ethan@example.com</v>
+      </c>
+      <c r="D63" t="str">
+        <v>Hialeah</v>
+      </c>
+      <c r="E63" t="str">
+        <v>FIU</v>
+      </c>
+      <c r="F63" t="str">
+        <v>Finance</v>
+      </c>
+      <c r="G63" t="str">
+        <v>Trader</v>
+      </c>
+      <c r="H63" t="str">
+        <v>Counselled</v>
+      </c>
+      <c r="I63" t="str">
+        <v>Explained fees</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>Farah Ali</v>
+      </c>
+      <c r="B64" t="str">
+        <v>+1-202-555-2048</v>
+      </c>
+      <c r="C64" t="str">
+        <v>farah@example.com</v>
+      </c>
+      <c r="D64" t="str">
+        <v>Garland</v>
+      </c>
+      <c r="E64" t="str">
+        <v>UNT</v>
+      </c>
+      <c r="F64" t="str">
+        <v>Marketing</v>
+      </c>
+      <c r="G64" t="str">
+        <v>Content Strategist</v>
+      </c>
+      <c r="H64" t="str">
+        <v>Enrolled</v>
+      </c>
+      <c r="I64" t="str">
+        <v>Orientation scheduled</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>George King</v>
+      </c>
+      <c r="B65" t="str">
+        <v>+1-202-555-2049</v>
+      </c>
+      <c r="C65" t="str">
+        <v>george@example.com</v>
+      </c>
+      <c r="D65" t="str">
+        <v>Scottsdale</v>
+      </c>
+      <c r="E65" t="str">
+        <v>ASU</v>
+      </c>
+      <c r="F65" t="str">
+        <v>Computer Science</v>
+      </c>
+      <c r="G65" t="str">
+        <v>Full-stack Dev</v>
+      </c>
+      <c r="H65" t="str">
+        <v>Buffer fresh</v>
+      </c>
+      <c r="I65" t="str">
+        <v>Awaiting email</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>Hana Suzuki</v>
+      </c>
+      <c r="B66" t="str">
+        <v>+1-202-555-2050</v>
+      </c>
+      <c r="C66" t="str">
+        <v>hana@example.com</v>
+      </c>
+      <c r="D66" t="str">
+        <v>Lubbock</v>
+      </c>
+      <c r="E66" t="str">
+        <v>TTU</v>
+      </c>
+      <c r="F66" t="str">
+        <v>Biology</v>
+      </c>
+      <c r="G66" t="str">
+        <v>Lab Tech</v>
+      </c>
+      <c r="H66" t="str">
+        <v>Request call back</v>
+      </c>
+      <c r="I66" t="str">
+        <v>Prefers morning</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>Ian McKay</v>
+      </c>
+      <c r="B67" t="str">
+        <v>+1-202-555-2051</v>
+      </c>
+      <c r="C67" t="str">
+        <v>ian@example.com</v>
+      </c>
+      <c r="D67" t="str">
+        <v>Chula Vista</v>
+      </c>
+      <c r="E67" t="str">
+        <v>SDSU</v>
+      </c>
+      <c r="F67" t="str">
+        <v>Data Science</v>
+      </c>
+      <c r="G67" t="str">
+        <v>ML Engineer</v>
+      </c>
+      <c r="H67" t="str">
+        <v>Interested in next batch</v>
+      </c>
+      <c r="I67" t="str">
+        <v>Waiting dates</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>Jia Huang</v>
+      </c>
+      <c r="B68" t="str">
+        <v>+1-202-555-2052</v>
+      </c>
+      <c r="C68" t="str">
+        <v>jia@example.com</v>
+      </c>
+      <c r="D68" t="str">
+        <v>Norfolk</v>
+      </c>
+      <c r="E68" t="str">
+        <v>ODU</v>
+      </c>
+      <c r="F68" t="str">
+        <v>Cybersecurity</v>
+      </c>
+      <c r="G68" t="str">
+        <v>Security Analyst</v>
+      </c>
+      <c r="H68" t="str">
+        <v>Registration fees paid</v>
+      </c>
+      <c r="I68" t="str">
+        <v>Paid online</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>Kabir Singh</v>
+      </c>
+      <c r="B69" t="str">
+        <v>+1-202-555-2053</v>
+      </c>
+      <c r="C69" t="str">
+        <v>kabir@example.com</v>
+      </c>
+      <c r="D69" t="str">
+        <v>Chesapeake</v>
+      </c>
+      <c r="E69" t="str">
+        <v>NSU</v>
+      </c>
+      <c r="F69" t="str">
+        <v>Economics</v>
+      </c>
+      <c r="G69" t="str">
+        <v>Research Associate</v>
+      </c>
+      <c r="H69" t="str">
+        <v>Follow up</v>
+      </c>
+      <c r="I69" t="str">
+        <v>Needs scholarship info</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>Lara Croft</v>
+      </c>
+      <c r="B70" t="str">
+        <v>+1-202-555-2054</v>
+      </c>
+      <c r="C70" t="str">
+        <v>lara@example.com</v>
+      </c>
+      <c r="D70" t="str">
+        <v>Durham</v>
+      </c>
+      <c r="E70" t="str">
+        <v>Duke</v>
+      </c>
+      <c r="F70" t="str">
+        <v>Anthropology</v>
+      </c>
+      <c r="G70" t="str">
+        <v>Field Researcher</v>
+      </c>
+      <c r="H70" t="str">
+        <v>Fresh</v>
+      </c>
+      <c r="I70" t="str">
+        <v>Initial interest</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>Mohammad Rahman</v>
+      </c>
+      <c r="B71" t="str">
+        <v>+1-202-555-2055</v>
+      </c>
+      <c r="C71" t="str">
+        <v>mohammad@example.com</v>
+      </c>
+      <c r="D71" t="str">
+        <v>Fort Wayne</v>
+      </c>
+      <c r="E71" t="str">
+        <v>Purdue Fort Wayne</v>
+      </c>
+      <c r="F71" t="str">
+        <v>IT</v>
+      </c>
+      <c r="G71" t="str">
+        <v>Network Engineer</v>
+      </c>
+      <c r="H71" t="str">
+        <v>Counselled</v>
+      </c>
+      <c r="I71" t="str">
+        <v>Compared tracks</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>Nina Lopez</v>
+      </c>
+      <c r="B72" t="str">
+        <v>+1-202-555-2056</v>
+      </c>
+      <c r="C72" t="str">
+        <v>nina@example.com</v>
+      </c>
+      <c r="D72" t="str">
+        <v>St. Paul</v>
+      </c>
+      <c r="E72" t="str">
+        <v>UMN</v>
+      </c>
+      <c r="F72" t="str">
+        <v>Psychology</v>
+      </c>
+      <c r="G72" t="str">
+        <v>Case Worker</v>
+      </c>
+      <c r="H72" t="str">
+        <v>Enrolled</v>
+      </c>
+      <c r="I72" t="str">
+        <v>Welcome email sent</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>Owen Parker</v>
+      </c>
+      <c r="B73" t="str">
+        <v>+1-202-555-2057</v>
+      </c>
+      <c r="C73" t="str">
+        <v>owen@example.com</v>
+      </c>
+      <c r="D73" t="str">
+        <v>Aurora</v>
+      </c>
+      <c r="E73" t="str">
+        <v>UC Denver</v>
+      </c>
+      <c r="F73" t="str">
+        <v>Architecture</v>
+      </c>
+      <c r="G73" t="str">
+        <v>CAD Specialist</v>
+      </c>
+      <c r="H73" t="str">
+        <v>Buffer fresh</v>
+      </c>
+      <c r="I73" t="str">
+        <v>Pending confirmation</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>Pari Mehta</v>
+      </c>
+      <c r="B74" t="str">
+        <v>+1-202-555-2058</v>
+      </c>
+      <c r="C74" t="str">
+        <v>pari@example.com</v>
+      </c>
+      <c r="D74" t="str">
+        <v>Jersey City</v>
+      </c>
+      <c r="E74" t="str">
+        <v>NJIT</v>
+      </c>
+      <c r="F74" t="str">
+        <v>Engineering</v>
+      </c>
+      <c r="G74" t="str">
+        <v>Process Engineer</v>
+      </c>
+      <c r="H74" t="str">
+        <v>Did not pick</v>
+      </c>
+      <c r="I74" t="str">
+        <v>Voicemail left</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>Rohan Desai</v>
+      </c>
+      <c r="B75" t="str">
+        <v>+1-202-555-2059</v>
+      </c>
+      <c r="C75" t="str">
+        <v>rohan@example.com</v>
+      </c>
+      <c r="D75" t="str">
+        <v>Irvine</v>
+      </c>
+      <c r="E75" t="str">
+        <v>UCI</v>
+      </c>
+      <c r="F75" t="str">
+        <v>MBA</v>
+      </c>
+      <c r="G75" t="str">
+        <v>Product Manager</v>
+      </c>
+      <c r="H75" t="str">
+        <v>Junk/not interested</v>
+      </c>
+      <c r="I75" t="str">
+        <v>Exploring other options</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K16"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I75"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>